<commit_message>
update finaly test single games
</commit_message>
<xml_diff>
--- a/static/media/df_prov.xlsx
+++ b/static/media/df_prov.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Jogos Gerados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,31 +437,13 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
-      </c>
-      <c r="C2" t="n">
-        <v>13</v>
-      </c>
-      <c r="D2" t="n">
-        <v>15</v>
-      </c>
-      <c r="E2" t="n">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -469,16 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -486,33 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>23</v>
-      </c>
-      <c r="E4" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>24</v>
-      </c>
-      <c r="C5" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" t="n">
-        <v>11</v>
-      </c>
-      <c r="E5" t="n">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update add col and del col
</commit_message>
<xml_diff>
--- a/static/media/df_prov.xlsx
+++ b/static/media/df_prov.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,16 +440,34 @@
       <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>90</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>87</v>
+      </c>
+      <c r="F2" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -457,10 +475,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3" t="n">
+        <v>43</v>
+      </c>
+      <c r="F3" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -468,10 +495,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="D4" t="n">
+        <v>55</v>
+      </c>
+      <c r="E4" t="n">
+        <v>42</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -479,10 +515,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="D5" t="n">
+        <v>28</v>
+      </c>
+      <c r="E5" t="n">
+        <v>49</v>
+      </c>
+      <c r="F5" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="6">
@@ -490,65 +535,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>16</v>
-      </c>
-      <c r="C7" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>11</v>
-      </c>
-      <c r="C8" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>21</v>
-      </c>
-      <c r="C9" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>14</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>16</v>
-      </c>
-      <c r="C11" t="n">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="D6" t="n">
+        <v>25</v>
+      </c>
+      <c r="E6" t="n">
+        <v>28</v>
+      </c>
+      <c r="F6" t="n">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>